<commit_message>
optimising the code of excel
</commit_message>
<xml_diff>
--- a/exceldownloadTest.xlsx
+++ b/exceldownloadTest.xlsx
@@ -28,7 +28,7 @@
     <t>season</t>
   </si>
   <si>
-    <t>Mango</t>
+    <t>Rabbit</t>
   </si>
   <si>
     <t>Yellow</t>
@@ -445,7 +445,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="0" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>